<commit_message>
Initial Wk 2 material
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A0374E-7056-0A41-9CEE-EC1082137530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790CAA2C-0C46-5F4D-A7FF-70F190D88B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>group</t>
   </si>
@@ -94,18 +94,9 @@
     <t>/example/01-example</t>
   </si>
   <si>
-    <t>/assignment/01-problem-set</t>
-  </si>
-  <si>
     <t>Weekly Topics</t>
   </si>
   <si>
-    <t>The Idea of a Shell: The terminal; finding, listing, and inspecting things</t>
-  </si>
-  <si>
-    <t>The Idea of Your Computer: The file system; naming things; the Unix way of thinking</t>
-  </si>
-  <si>
     <t>The Idea of Plain Text: Text editors; slicing and dicing; regular expressions</t>
   </si>
   <si>
@@ -116,6 +107,18 @@
   </si>
   <si>
     <t>The Idea of the Network: Servers, websites, and APIs</t>
+  </si>
+  <si>
+    <t>The Idea of Your Computer: The file system; the terminal; the Unix way of thinking</t>
+  </si>
+  <si>
+    <t>The Idea of a Shell: Finding, listing, and inspecting things</t>
+  </si>
+  <si>
+    <t>/content/02-content</t>
+  </si>
+  <si>
+    <t>/example/02-example</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +494,7 @@
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="1"/>
     <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -534,7 +537,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -545,7 +548,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
@@ -553,13 +556,10 @@
       <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -570,12 +570,18 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -586,12 +592,12 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -602,12 +608,12 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -618,12 +624,12 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -634,7 +640,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3"/>
     </row>

</xml_diff>

<commit_message>
More wk 2 material
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790CAA2C-0C46-5F4D-A7FF-70F190D88B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C360639-252A-8949-87B3-2FD1CCD0C77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>group</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>/example/02-example</t>
+  </si>
+  <si>
+    <t>/assignment/02-problem-set</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,6 +581,9 @@
       <c r="I3" t="s">
         <v>27</v>
       </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
More wk01, data sources list
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B745D083-1EE6-C849-9FC3-154228BA7079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B349CDC-5AAE-F948-865E-BD8C2701A6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3520" windowWidth="33540" windowHeight="16460" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>No class (Thanksgiving)</t>
   </si>
   <si>
-    <t>Doing data analysis properly</t>
-  </si>
-  <si>
     <t>Your computer: The file system; the terminal; the Unix way of thinking</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>/assignment/01-assignment</t>
+  </si>
+  <si>
+    <t>Big Picture: Doing your work properly</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,16 +598,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -639,7 +639,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -655,7 +655,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -671,7 +671,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -687,7 +687,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -704,7 +704,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -737,7 +737,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -754,7 +754,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -771,7 +771,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -787,7 +787,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -804,7 +804,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H14" s="3"/>
     </row>

</xml_diff>

<commit_message>
Much more (too much) material on files
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786C36F3-B450-A64C-9873-23545B107222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2D8E33-E9A6-F846-AFD5-C4043BEE2420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3520" windowWidth="33540" windowHeight="16460" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -150,9 +150,6 @@
     <t>Your data workbench II: How R thinks; tidy data</t>
   </si>
   <si>
-    <t>Reproducible data: build systems, environments, and packages</t>
-  </si>
-  <si>
     <t>/content/01-content</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Big Picture: Doing your work properly</t>
+  </si>
+  <si>
+    <t>Reproducible results: build systems, environments, and packages</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,16 +598,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3"/>
     </row>

</xml_diff>

<commit_message>
wk01 slides; wk02 updates
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2D8E33-E9A6-F846-AFD5-C4043BEE2420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717243A-455B-9640-AF36-FAEC89AC49FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3520" windowWidth="33540" windowHeight="16460" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>group</t>
   </si>
@@ -120,15 +120,6 @@
     <t>No class (Thanksgiving)</t>
   </si>
   <si>
-    <t>Your computer: The file system; the terminal; the Unix way of thinking</t>
-  </si>
-  <si>
-    <t>The shell: Finding, listing, and inspecting things</t>
-  </si>
-  <si>
-    <t>Editing text: Text editors; slicing and dicing; regular expressions</t>
-  </si>
-  <si>
     <t>Your data workbench I: R, RStudio, and Quarto</t>
   </si>
   <si>
@@ -163,6 +154,21 @@
   </si>
   <si>
     <t>Reproducible results: build systems, environments, and packages</t>
+  </si>
+  <si>
+    <t>The file system; the shell; the terminal</t>
+  </si>
+  <si>
+    <t>Editing text: Text editors; regular expressions</t>
+  </si>
+  <si>
+    <t>/content/02-content</t>
+  </si>
+  <si>
+    <t>/example/02-example</t>
+  </si>
+  <si>
+    <t>/assignment/02-assignment</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,16 +604,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -623,7 +629,16 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -639,7 +654,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -655,7 +670,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -671,7 +686,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -687,7 +702,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -704,7 +719,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -720,7 +735,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -737,7 +752,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H10" s="3"/>
     </row>
@@ -754,7 +769,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H11" s="3"/>
     </row>
@@ -771,7 +786,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -787,7 +802,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="H13" s="3"/>
     </row>
@@ -803,9 +818,6 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add final wk's slides, finally
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11103"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB008BE-EE30-1545-A0D7-1D2BF5B2DAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216F8FCE-FE1A-F947-88A3-9C47756ABD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3520" windowWidth="33540" windowHeight="16460" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
   <si>
     <t>group</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>/content/11-content</t>
+  </si>
+  <si>
+    <t>/content/12-content</t>
+  </si>
+  <si>
+    <t>/example/11-example</t>
   </si>
 </sst>
 </file>
@@ -620,7 +626,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -954,6 +960,9 @@
       <c r="H13" t="s">
         <v>70</v>
       </c>
+      <c r="I13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -970,7 +979,9 @@
       <c r="F14" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Rearrange dt Labor Day; fix layout issues
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCCF41B2-200C-CC4A-8144-9CAF30A19FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2517DD13-1432-4C4C-BC2F-047C20202A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3520" windowWidth="33540" windowHeight="16460" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -114,42 +114,18 @@
     <t>No class (Fall break)</t>
   </si>
   <si>
-    <t>Your data workbench I: R, RStudio, and Quarto</t>
-  </si>
-  <si>
     <t>Version Control: git and GitHub</t>
   </si>
   <si>
-    <t>Iterate on data: functional programming patterns</t>
-  </si>
-  <si>
-    <t>Look at data: Graphs, ggplot, and the grammar of graphics</t>
-  </si>
-  <si>
-    <t>Your data workbench II: How R thinks; tidy data</t>
-  </si>
-  <si>
     <t>Big Picture: Doing your work properly</t>
   </si>
   <si>
-    <t>Reproducible results: build systems, environments, and packages</t>
-  </si>
-  <si>
     <t>The file system; the shell; the terminal</t>
   </si>
   <si>
-    <t>Editing text: Text editors; regular expressions</t>
-  </si>
-  <si>
-    <t>Ingest data: Getting stuff in and out of R</t>
-  </si>
-  <si>
     <t>example</t>
   </si>
   <si>
-    <t xml:space="preserve">Supercharged iteration: Parallel computing </t>
-  </si>
-  <si>
     <t>Databases and APIs</t>
   </si>
   <si>
@@ -162,7 +138,31 @@
     <t>/example/01-example-oecd</t>
   </si>
   <si>
-    <t>/assignment/01-assignment-install-r-github</t>
+    <t>/assignment/01-assignment-quarto-notes</t>
+  </si>
+  <si>
+    <t>No class (Labor Day)</t>
+  </si>
+  <si>
+    <t>Using R to look at data</t>
+  </si>
+  <si>
+    <t>Working with models</t>
+  </si>
+  <si>
+    <t>Functional programming patterns</t>
+  </si>
+  <si>
+    <t>Ingesting and cleaning data</t>
+  </si>
+  <si>
+    <t>Tidy data and dplyr</t>
+  </si>
+  <si>
+    <t>Build systems, environments, and packages</t>
+  </si>
+  <si>
+    <t>Better tables, better graphs</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
         <v>7</v>
@@ -598,16 +598,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J3" s="3"/>
     </row>
@@ -640,7 +640,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3"/>
     </row>
@@ -657,7 +657,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J5" s="3"/>
     </row>
@@ -674,7 +674,7 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J6" s="3"/>
     </row>
@@ -691,7 +691,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J7" s="3"/>
     </row>
@@ -708,7 +708,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J8" s="3"/>
     </row>
@@ -742,7 +742,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" s="3"/>
     </row>
@@ -759,7 +759,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="3"/>
     </row>
@@ -776,7 +776,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J12" s="3"/>
     </row>
@@ -793,7 +793,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -809,7 +809,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -825,7 +825,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H15" s="3"/>
     </row>

</xml_diff>

<commit_message>
quarto 1.8 updates and fixes
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/mptc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E66A73C-ABBF-DD43-8E93-C08E67CEF9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDEFA5C-35C4-DE44-84C3-24C52E881B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10660" yWindow="2800" windowWidth="23900" windowHeight="18380" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -201,10 +201,10 @@
     <t>/content/07-content-ingesting-data</t>
   </si>
   <si>
-    <t>assignment/07-assignment-fars</t>
-  </si>
-  <si>
-    <t>/example/05-example-dplyr-and-more</t>
+    <t>/example/06-example-dplyr-and-more</t>
+  </si>
+  <si>
+    <t>/assignment/07-assignment-fars</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,7 +766,7 @@
         <v>53</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J7" s="3"/>
     </row>
@@ -789,7 +789,7 @@
         <v>54</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>